<commit_message>
Extraction rule is coded, Team Id is used for Editing and deleting Team. Also, validation on deleting is added.  AdministrationTeamCRUD.webtest.
</commit_message>
<xml_diff>
--- a/Lista testova za Regression test.xlsx
+++ b/Lista testova za Regression test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="20010" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
   <si>
     <t>LISTA TESTOVA ZA REGRESSION TEST</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Invalid login   - username</t>
   </si>
   <si>
-    <t>LoginInvalidUserName</t>
-  </si>
-  <si>
     <t>Invalid login   - password</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
   </si>
   <si>
     <t>Pogresno korisnicko ime, poruka ista kao I kada je pogresna lozinka</t>
-  </si>
-  <si>
-    <t>LoginInvalidPassword</t>
   </si>
   <si>
     <t>Forgotten password - correct mail address</t>
@@ -485,6 +479,9 @@
   </si>
   <si>
     <t>SubmissionDetailpageAuthorised approvers</t>
+  </si>
+  <si>
+    <t>LoginInvalidCredentials</t>
   </si>
 </sst>
 </file>
@@ -854,7 +851,7 @@
   <dimension ref="A2:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,10 +901,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -915,13 +912,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,13 +926,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -943,13 +940,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -957,13 +954,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -971,13 +968,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -985,13 +982,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -999,13 +996,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1013,13 +1010,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1027,13 +1024,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1041,13 +1038,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1055,13 +1052,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1069,13 +1066,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1083,13 +1080,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1097,13 +1094,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1111,13 +1108,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1125,13 +1122,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1139,13 +1136,13 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1153,13 +1150,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1167,13 +1164,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1181,13 +1178,13 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1195,13 +1192,13 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1209,13 +1206,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1223,13 +1220,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1237,13 +1234,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1251,13 +1248,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1265,13 +1262,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1279,13 +1276,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1293,13 +1290,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1307,13 +1304,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1321,13 +1318,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1335,13 +1332,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1349,13 +1346,13 @@
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1363,13 +1360,13 @@
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1377,13 +1374,13 @@
         <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1391,13 +1388,13 @@
         <v>37</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1405,13 +1402,13 @@
         <v>38</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Dodana jos dva testa na stranici Preference za testianje Certification of deed dela da li da se pojavljuje odmah ili tek pred Submit to CH
</commit_message>
<xml_diff>
--- a/Lista testova za Regression test.xlsx
+++ b/Lista testova za Regression test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="142">
   <si>
     <t>LISTA TESTOVA ZA REGRESSION TEST</t>
   </si>
@@ -103,12 +103,6 @@
   </si>
   <si>
     <t>Administration Preferences Edit</t>
-  </si>
-  <si>
-    <t>Provera izmene postavke na Preferences stranici bez promene statusa iz TEST u LIVE</t>
-  </si>
-  <si>
-    <t>AdministrationPreferencesEdit</t>
   </si>
   <si>
     <t>Administration Reports</t>
@@ -488,6 +482,81 @@
   </si>
   <si>
     <t>Dobijanje liste korisnika, izmena prikaza broja redova, skok na sledecu stranicu, vracanje na prethodnu , search, skok na poslednju stranicu</t>
+  </si>
+  <si>
+    <t>10.a</t>
+  </si>
+  <si>
+    <t>10.b</t>
+  </si>
+  <si>
+    <t>10.c</t>
+  </si>
+  <si>
+    <t>10.d</t>
+  </si>
+  <si>
+    <t>10.e</t>
+  </si>
+  <si>
+    <t>10.f</t>
+  </si>
+  <si>
+    <t>10.g</t>
+  </si>
+  <si>
+    <t>10.h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LISTA TESTOVA KOJA TESTIRA POJEDINACNE STETINGSE </t>
+  </si>
+  <si>
+    <t>Provera da li se za MR01 I MR02 javlja unos licnih podataka tek kada se salje upit prema CH</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesCertificateAtPoint</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesRedactionStatement</t>
+  </si>
+  <si>
+    <t>Provera da li se podatak o Redaction Satetmentu prenosi kao parametar za MR01 I MR02</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka za URGENT days odrazava kod kreiranja MR01</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesUrgentDay</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka za VERY URGENT days odrazava kod kreiranja MR01</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesVeryUrgentDay</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka za ARCHIVE days odrazava kod odobrenih od strane CH  MR01</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesArchiveDay</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka JOB reference odrazava kod kreiranja submissiona</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesJobReference</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka Client matter visible odrazava kod kreiranja submissiona</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesClientMatterVisible</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka Client matter required odrazava kod kreiranja submissiona</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesClientMatterRequired</t>
   </si>
 </sst>
 </file>
@@ -1102,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G42"/>
+  <dimension ref="A2:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,18 +1182,18 @@
     <col min="1" max="1" width="6.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="18" t="s">
         <v>1</v>
@@ -1136,10 +1205,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>1</v>
       </c>
@@ -1153,10 +1222,10 @@
         <v>6</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -1167,13 +1236,13 @@
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>3</v>
       </c>
@@ -1184,13 +1253,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>4</v>
       </c>
@@ -1204,10 +1273,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>5</v>
       </c>
@@ -1221,13 +1290,10 @@
         <v>12</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G9" s="1">
-        <v>144.976</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>6</v>
       </c>
@@ -1241,13 +1307,10 @@
         <v>18</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="1">
-        <v>123.86750000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>7</v>
       </c>
@@ -1261,14 +1324,10 @@
         <v>22</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" s="1">
-        <f>G9/G10</f>
-        <v>1.17041193210487</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>8</v>
       </c>
@@ -1276,16 +1335,16 @@
         <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>9</v>
       </c>
@@ -1298,9 +1357,11 @@
       <c r="D13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>10</v>
       </c>
@@ -1308,432 +1369,534 @@
         <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="23"/>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="23"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E20" s="23"/>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="23"/>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="23"/>
+    </row>
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>11</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="23"/>
-    </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>11</v>
-      </c>
-      <c r="B15" s="5" t="s">
+      <c r="D23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="E23" s="23"/>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>12</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="C24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>12</v>
-      </c>
-      <c r="B16" s="5" t="s">
+      <c r="D24" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="E24" s="23"/>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>13</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="C25" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="23"/>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>13</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="D25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>14</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="C26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
-        <v>14</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="E26" s="23"/>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>15</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="C27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="23"/>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>15</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="D27" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>16</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="23"/>
-    </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
-        <v>17</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="23"/>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
-        <v>18</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="23"/>
-    </row>
-    <row r="23" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>19</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="23"/>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
-        <v>20</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" s="23"/>
-    </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
-        <v>21</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>22</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="7">
-        <v>23</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>77</v>
       </c>
       <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E28" s="23"/>
     </row>
-    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E30" s="23"/>
     </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>20</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="E32" s="23"/>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>21</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="23"/>
-    </row>
-    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="7">
-        <v>28</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="23"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
-        <v>29</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="E34" s="23"/>
     </row>
-    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="E36" s="23"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="E37" s="23"/>
     </row>
     <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
+        <v>26</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>27</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39" s="23"/>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>28</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="23"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>29</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="23"/>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>30</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" s="23"/>
+    </row>
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>31</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="23"/>
+    </row>
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>32</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E44" s="23"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>33</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="23"/>
+    </row>
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <v>34</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B46" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" s="23"/>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>35</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E47" s="23"/>
+    </row>
+    <row r="48" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>36</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="23"/>
-    </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
-        <v>35</v>
-      </c>
-      <c r="B39" s="5" t="s">
+      <c r="D48" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E48" s="23"/>
+    </row>
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>37</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="23"/>
-    </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="7">
-        <v>36</v>
-      </c>
-      <c r="B40" s="5" t="s">
+      <c r="E49" s="23"/>
+    </row>
+    <row r="50" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="9">
+        <v>38</v>
+      </c>
+      <c r="B50" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C50" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D50" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="23"/>
-    </row>
-    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
-        <v>37</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E41" s="23"/>
-    </row>
-    <row r="42" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9">
-        <v>38</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" s="24"/>
+      <c r="E50" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Radjeno na proveri unosa podataka na Preferences stranici za Urgent days
</commit_message>
<xml_diff>
--- a/Lista testova za Regression test.xlsx
+++ b/Lista testova za Regression test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="142">
   <si>
     <t>LISTA TESTOVA ZA REGRESSION TEST</t>
   </si>
@@ -514,9 +514,6 @@
     <t>Provera da li se za MR01 I MR02 javlja unos licnih podataka tek kada se salje upit prema CH</t>
   </si>
   <si>
-    <t>AdministrationPreferencesCertificateAtPoint</t>
-  </si>
-  <si>
     <t>AdministrationPreferencesRedactionStatement</t>
   </si>
   <si>
@@ -557,6 +554,10 @@
   </si>
   <si>
     <t>AdministrationPreferencesClientMatterRequired</t>
+  </si>
+  <si>
+    <t>AdministrationPreferencesCertificateAtPoint-FALSE
+AdministrationPreferencesCertificateAtPoint-TRUE</t>
   </si>
 </sst>
 </file>
@@ -796,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -869,6 +870,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1186,7 @@
     <col min="1" max="1" width="6.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1382,10 +1386,12 @@
       <c r="C15" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E15" s="23"/>
+      <c r="D15" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -1393,12 +1399,14 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E16" s="23"/>
+        <v>127</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -1406,10 +1414,10 @@
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="E17" s="23"/>
     </row>
@@ -1419,10 +1427,10 @@
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>133</v>
       </c>
       <c r="E18" s="23"/>
     </row>
@@ -1432,10 +1440,10 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>134</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>135</v>
       </c>
       <c r="E19" s="23"/>
     </row>
@@ -1445,10 +1453,10 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>136</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="E20" s="23"/>
     </row>
@@ -1458,10 +1466,10 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="E21" s="23"/>
     </row>
@@ -1471,10 +1479,10 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>140</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>141</v>
       </c>
       <c r="E22" s="23"/>
     </row>

</xml_diff>

<commit_message>
Dodano nekoliko testova jos, nedovrsen je dio vezan za validaciju panela na MyDasboard stranici  i na tome se radi.
</commit_message>
<xml_diff>
--- a/Lista testova za Regression test.xlsx
+++ b/Lista testova za Regression test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="144">
   <si>
     <t>LISTA TESTOVA ZA REGRESSION TEST</t>
   </si>
@@ -108,16 +108,10 @@
     <t>Administration Reports</t>
   </si>
   <si>
-    <t>Provera valjanosti podataka na reportu. Test raditi tako da se prvo utvrdi koliko ima odobrenih submissiona preko Global Submission liste a onda praviti poredjenje sa onim sto je prikazanao na Report stranici</t>
-  </si>
-  <si>
     <t>AdministrationReport</t>
   </si>
   <si>
     <t>Administration Submissions reliant on CH</t>
-  </si>
-  <si>
-    <t>Provera broja submitovanih submissiona na CH bez odziva CH I nakon toga provera da li taj broj odgovara onome sto se pojavljuje na ovoj stranici</t>
   </si>
   <si>
     <t>AdministrationReliant</t>
@@ -520,25 +514,13 @@
     <t>Provera da li se podatak o Redaction Satetmentu prenosi kao parametar za MR01 I MR02</t>
   </si>
   <si>
-    <t>Provera da li se postavka za URGENT days odrazava kod kreiranja MR01</t>
-  </si>
-  <si>
     <t>AdministrationPreferencesUrgentDay</t>
   </si>
   <si>
-    <t>Provera da li se postavka za VERY URGENT days odrazava kod kreiranja MR01</t>
-  </si>
-  <si>
     <t>AdministrationPreferencesVeryUrgentDay</t>
   </si>
   <si>
-    <t>Provera da li se postavka za ARCHIVE days odrazava kod odobrenih od strane CH  MR01</t>
-  </si>
-  <si>
     <t>AdministrationPreferencesArchiveDay</t>
-  </si>
-  <si>
-    <t>Provera da li se postavka JOB reference odrazava kod kreiranja submissiona</t>
   </si>
   <si>
     <t>AdministrationPreferencesJobReference</t>
@@ -558,6 +540,30 @@
   <si>
     <t>AdministrationPreferencesCertificateAtPoint-FALSE
 AdministrationPreferencesCertificateAtPoint-TRUE</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Provera da li se postavka za ARCHIVE days odrazava kod odobrenih od strane CH  MR01. NE MOGU DA NAPRAVIM TEST CASE JER NE MOGU DA BUDEM SIGURAN DA IMA APPROVED SUBMISSIONS U BAZI. OSTAVLJAM GA ZA SADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provera da li se postavka za URGENT days odrazava kod kreiranja MR01. Definisem ulazne parametre na Prefrences stranici. Kreiram MR01 tako da budu zadovoljeni uslovi da se datumi uklapaju. Proveravam da li je attribut class= "urgent " dodan u tabeli gde se prikazuju svi submissioni. Moguce je da se isti test ponovi sa istim ulaznim parametrima ali da se Charge ceation date postavi tako da ne ulazi u opseg datuma. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provera da li se postavka za VERY URGENT days odrazava kod kreiranja MR01.Kreiram MR01 tako da budu zadovoljeni uslovi da se datumi uklapaju. Proveravam da li je attribut class= "urgent " dodan u tabeli gde se prikazuju svi submissioni. Moguce je da se isti test ponovi sa istim ulaznim parametrima ali da se Charge ceation date postavi tako da ne ulazi u opseg datuma. </t>
+  </si>
+  <si>
+    <t>Provera da li se postavka JOB reference odrazava kod kreiranja submissiona. Skidam Client matter number I postavljam JOB refernce a onda idem na kreiranje novog submissiona I proveravam da li se pojavljuje poruka za obavezan unos job reference.</t>
+  </si>
+  <si>
+    <t>Provera valjanosti podataka na reportu. Test raditi tako da se prvo utvrdi koliko ima odobrenih submissiona preko Global Submission liste a onda praviti poredjenje sa onim sto je prikazanao na Report stranici. OSTAVITI ZA KASNIJE, LOGIKA JE DOSTA PROBLEMATICNA, JER SE NE PRIKAZUJU SVI APPROVED BY CH SUBMISSIONI NA GLOBAL SUBMISSION LISTI I MORALO BI DA SE IDE U BAZU I IZ BAZE CITAJU OCEKIVANI REZULTATI</t>
+  </si>
+  <si>
+    <t>LATTER</t>
+  </si>
+  <si>
+    <t>Provera broja submitovanih submissiona na CH bez odziva CH I nakon toga provera da li taj broj odgovara onome sto se pojavljuje na ovoj stranici. Ideja je da se kreira jedan submission I da se posalje prema CH, a onda da se potrazi da li postoji u jednoj ili drugoj tabeli koje su prikazane i ako se pojavi , test je prosao.</t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1226,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1240,10 +1246,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1257,10 +1263,10 @@
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>113</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,7 +1283,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1294,7 +1300,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1311,7 +1317,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1328,7 +1334,7 @@
         <v>22</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1339,13 +1345,13 @@
         <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1362,7 +1368,7 @@
         <v>26</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1373,120 +1379,132 @@
         <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E17" s="23"/>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="23"/>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="23"/>
-    </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E20" s="23"/>
+        <v>130</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E21" s="23"/>
+        <v>132</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E22" s="23"/>
-    </row>
-    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>11</v>
       </c>
@@ -1494,25 +1512,27 @@
         <v>29</v>
       </c>
       <c r="C23" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="23"/>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E23" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>12</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="E24" s="23"/>
     </row>
@@ -1521,13 +1541,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="E25" s="23"/>
     </row>
@@ -1536,13 +1556,13 @@
         <v>14</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="E26" s="23"/>
     </row>
@@ -1551,13 +1571,13 @@
         <v>15</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>43</v>
       </c>
       <c r="E27" s="23"/>
     </row>
@@ -1566,13 +1586,13 @@
         <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E28" s="23"/>
     </row>
@@ -1581,13 +1601,13 @@
         <v>17</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E29" s="23"/>
     </row>
@@ -1596,13 +1616,13 @@
         <v>18</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E30" s="23"/>
     </row>
@@ -1611,13 +1631,13 @@
         <v>19</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E31" s="23"/>
     </row>
@@ -1626,13 +1646,13 @@
         <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E32" s="23"/>
     </row>
@@ -1641,13 +1661,13 @@
         <v>21</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E33" s="23"/>
     </row>
@@ -1656,13 +1676,13 @@
         <v>22</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E34" s="23"/>
     </row>
@@ -1671,13 +1691,13 @@
         <v>23</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E35" s="23"/>
     </row>
@@ -1686,13 +1706,13 @@
         <v>24</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E36" s="23"/>
     </row>
@@ -1701,13 +1721,13 @@
         <v>25</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E37" s="23"/>
     </row>
@@ -1716,13 +1736,13 @@
         <v>26</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E38" s="23"/>
     </row>
@@ -1731,13 +1751,13 @@
         <v>27</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E39" s="23"/>
     </row>
@@ -1746,13 +1766,13 @@
         <v>28</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="8" t="s">
         <v>80</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>82</v>
       </c>
       <c r="E40" s="23"/>
     </row>
@@ -1761,13 +1781,13 @@
         <v>29</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="E41" s="23"/>
     </row>
@@ -1776,13 +1796,13 @@
         <v>30</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E42" s="23"/>
     </row>
@@ -1791,13 +1811,13 @@
         <v>31</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E43" s="23"/>
     </row>
@@ -1806,13 +1826,13 @@
         <v>32</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E44" s="23"/>
     </row>
@@ -1821,13 +1841,13 @@
         <v>33</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E45" s="23"/>
     </row>
@@ -1836,13 +1856,13 @@
         <v>34</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E46" s="23"/>
     </row>
@@ -1851,13 +1871,13 @@
         <v>35</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E47" s="23"/>
     </row>
@@ -1866,13 +1886,13 @@
         <v>36</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E48" s="23"/>
     </row>
@@ -1881,13 +1901,13 @@
         <v>37</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E49" s="23"/>
     </row>
@@ -1896,13 +1916,13 @@
         <v>38</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E50" s="24"/>
     </row>

</xml_diff>